<commit_message>
Continuação do módulo 4 - Autopreenchimento e validação de dados
</commit_message>
<xml_diff>
--- a/Modulo 4 - Mais tópicos de edição e formatação/aula-autopreenchimento.xlsx
+++ b/Modulo 4 - Mais tópicos de edição e formatação/aula-autopreenchimento.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\04 Mais tópicos de edição e formatação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarketTi\Desktop\Curso-Excel\Modulo 4 - Mais tópicos de edição e formatação\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD89600-E1F0-4248-A4C4-EEE352B3CE56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
     <sheet name="Lançamentos" sheetId="2" r:id="rId2"/>
     <sheet name="Relatórios" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Dia</t>
   </si>
@@ -75,11 +76,47 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Janeiro</t>
+  </si>
+  <si>
+    <t>Fevereiro</t>
+  </si>
+  <si>
+    <t>Março</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Maio</t>
+  </si>
+  <si>
+    <t>Junho</t>
+  </si>
+  <si>
+    <t>Julho</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Setembro</t>
+  </si>
+  <si>
+    <t>Outubro</t>
+  </si>
+  <si>
+    <t>Novembro</t>
+  </si>
+  <si>
+    <t>Dezembro</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
@@ -568,7 +605,7 @@
         <xdr:cNvPr id="8" name="Retângulo: Único Canto Recortado 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{68D92666-11B7-401A-B465-5FF5EE91444B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D92666-11B7-401A-B465-5FF5EE91444B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -647,7 +684,7 @@
         <xdr:cNvPr id="16" name="Imagem 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DD455D8-DD2E-4E47-A793-02EFDF9CAC96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DD455D8-DD2E-4E47-A793-02EFDF9CAC96}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -690,7 +727,7 @@
         <xdr:cNvPr id="17" name="CaixaDeTexto 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88F505DC-0525-4B37-B8DC-24B423530C24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88F505DC-0525-4B37-B8DC-24B423530C24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -776,7 +813,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61A5EA32-C5C9-47A5-A9FE-68ABE8608E4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A5EA32-C5C9-47A5-A9FE-68ABE8608E4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -854,7 +891,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F6DEA5C-FE02-4F70-AC4E-521F970DE373}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6DEA5C-FE02-4F70-AC4E-521F970DE373}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -937,7 +974,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{28257CA3-3903-423C-A6C2-F683C2E40B89}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28257CA3-3903-423C-A6C2-F683C2E40B89}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1015,7 +1052,7 @@
         <xdr:cNvPr id="4" name="CaixaDeTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5BDCDB88-ABAD-4D9C-B688-EE9AF895B4B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BDCDB88-ABAD-4D9C-B688-EE9AF895B4B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1100,7 +1137,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Único Canto Recortado 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5313F8A0-0508-40E1-BF8F-DE0267486572}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5313F8A0-0508-40E1-BF8F-DE0267486572}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1181,7 +1218,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{75B69EAC-656C-43AB-8420-BB7D0198B779}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B69EAC-656C-43AB-8420-BB7D0198B779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1264,7 +1301,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{74767F19-F1BF-440F-AFCD-DD07336FB9A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74767F19-F1BF-440F-AFCD-DD07336FB9A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1342,7 +1379,7 @@
         <xdr:cNvPr id="4" name="CaixaDeTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF2D846A-C8E7-49BD-9759-CB65C0C90D7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF2D846A-C8E7-49BD-9759-CB65C0C90D7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1428,7 +1465,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3D06FE2-47E5-4094-A4BF-3D513125E10F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3D06FE2-47E5-4094-A4BF-3D513125E10F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1505,7 +1542,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Único Canto Recortado 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{01B27A03-A007-472D-9845-C8D9BE715F5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B27A03-A007-472D-9845-C8D9BE715F5C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1866,20 +1903,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="16384" width="11.7109375" hidden="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="16" width="11.7265625" customWidth="1"/>
+    <col min="17" max="17" width="3.7265625" customWidth="1"/>
+    <col min="18" max="16384" width="11.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -1896,7 +1933,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1913,7 +1950,7 @@
       <c r="O2" s="15"/>
       <c r="P2" s="16"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1930,7 +1967,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1947,7 +1984,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1964,7 +2001,7 @@
       <c r="O5" s="6"/>
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1981,7 +2018,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="7"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1998,7 +2035,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="2:16" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:16" ht="17" x14ac:dyDescent="0.5">
       <c r="B8" s="5"/>
       <c r="C8" s="17"/>
       <c r="D8" s="6"/>
@@ -2015,7 +2052,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="7"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -2032,7 +2069,7 @@
       <c r="O9" s="6"/>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -2049,7 +2086,7 @@
       <c r="O10" s="6"/>
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -2066,7 +2103,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="7"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -2083,7 +2120,7 @@
       <c r="O12" s="6"/>
       <c r="P12" s="7"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2100,7 +2137,7 @@
       <c r="O13" s="6"/>
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2117,7 +2154,7 @@
       <c r="O14" s="6"/>
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2134,7 +2171,7 @@
       <c r="O15" s="6"/>
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2151,7 +2188,7 @@
       <c r="O16" s="6"/>
       <c r="P16" s="7"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2168,7 +2205,7 @@
       <c r="O17" s="6"/>
       <c r="P17" s="7"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2185,7 +2222,7 @@
       <c r="O18" s="6"/>
       <c r="P18" s="7"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -2202,7 +2239,7 @@
       <c r="O19" s="6"/>
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -2219,7 +2256,7 @@
       <c r="O20" s="6"/>
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -2236,7 +2273,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="7"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2260,20 +2297,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="51" customWidth="1"/>
-    <col min="2" max="16" width="11.7109375" style="51" customWidth="1"/>
-    <col min="17" max="17" width="3.7109375" style="51" customWidth="1"/>
-    <col min="18" max="16384" width="11.7109375" style="51" hidden="1"/>
+    <col min="1" max="1" width="3.7265625" style="51" customWidth="1"/>
+    <col min="2" max="16" width="11.7265625" style="51" customWidth="1"/>
+    <col min="17" max="17" width="3.7265625" style="51" customWidth="1"/>
+    <col min="18" max="16384" width="11.7265625" style="51" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="44" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" s="44" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="41"/>
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
@@ -2290,7 +2329,7 @@
       <c r="O1" s="42"/>
       <c r="P1" s="43"/>
     </row>
-    <row r="2" spans="2:16" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="45"/>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -2307,7 +2346,7 @@
       <c r="O2" s="46"/>
       <c r="P2" s="47"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="48"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
@@ -2324,7 +2363,7 @@
       <c r="O3" s="49"/>
       <c r="P3" s="50"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="52"/>
       <c r="C4" s="53" t="s">
         <v>9</v>
@@ -2349,7 +2388,7 @@
       <c r="O4" s="79"/>
       <c r="P4" s="80"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="52"/>
       <c r="C5" s="58" t="s">
         <v>0</v>
@@ -2382,16 +2421,20 @@
       <c r="O5" s="79"/>
       <c r="P5" s="80"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="52"/>
-      <c r="C6" s="61"/>
+      <c r="C6" s="61">
+        <v>43374</v>
+      </c>
       <c r="D6" s="62"/>
       <c r="E6" s="62"/>
       <c r="F6" s="63">
         <v>950</v>
       </c>
       <c r="G6" s="56"/>
-      <c r="H6" s="77"/>
+      <c r="H6" s="77">
+        <v>1</v>
+      </c>
       <c r="I6" s="62">
         <v>249</v>
       </c>
@@ -2406,9 +2449,11 @@
       <c r="O6" s="79"/>
       <c r="P6" s="80"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="52"/>
-      <c r="C7" s="64"/>
+      <c r="C7" s="64">
+        <v>43375</v>
+      </c>
       <c r="D7" s="65"/>
       <c r="E7" s="65">
         <v>200</v>
@@ -2418,7 +2463,9 @@
         <v>750</v>
       </c>
       <c r="G7" s="56"/>
-      <c r="H7" s="78"/>
+      <c r="H7" s="78">
+        <v>2</v>
+      </c>
       <c r="I7" s="65">
         <v>600</v>
       </c>
@@ -2433,9 +2480,11 @@
       <c r="O7" s="79"/>
       <c r="P7" s="80"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="52"/>
-      <c r="C8" s="64"/>
+      <c r="C8" s="64">
+        <v>43376</v>
+      </c>
       <c r="D8" s="65"/>
       <c r="E8" s="65">
         <v>250</v>
@@ -2445,7 +2494,9 @@
         <v>500</v>
       </c>
       <c r="G8" s="56"/>
-      <c r="H8" s="78"/>
+      <c r="H8" s="78">
+        <v>3</v>
+      </c>
       <c r="I8" s="65"/>
       <c r="J8" s="65">
         <v>25</v>
@@ -2460,9 +2511,11 @@
       <c r="O8" s="79"/>
       <c r="P8" s="80"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="52"/>
-      <c r="C9" s="64"/>
+      <c r="C9" s="64">
+        <v>43377</v>
+      </c>
       <c r="D9" s="65"/>
       <c r="E9" s="65">
         <v>95</v>
@@ -2472,7 +2525,9 @@
         <v>405</v>
       </c>
       <c r="G9" s="56"/>
-      <c r="H9" s="78"/>
+      <c r="H9" s="78">
+        <v>4</v>
+      </c>
       <c r="I9" s="65"/>
       <c r="J9" s="65">
         <v>39</v>
@@ -2487,9 +2542,11 @@
       <c r="O9" s="79"/>
       <c r="P9" s="80"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="52"/>
-      <c r="C10" s="64"/>
+      <c r="C10" s="64">
+        <v>43378</v>
+      </c>
       <c r="D10" s="65"/>
       <c r="E10" s="65">
         <v>156</v>
@@ -2499,7 +2556,9 @@
         <v>249</v>
       </c>
       <c r="G10" s="56"/>
-      <c r="H10" s="78"/>
+      <c r="H10" s="78">
+        <v>5</v>
+      </c>
       <c r="I10" s="65"/>
       <c r="J10" s="65">
         <v>10</v>
@@ -2514,9 +2573,11 @@
       <c r="O10" s="79"/>
       <c r="P10" s="80"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" s="52"/>
-      <c r="C11" s="64"/>
+      <c r="C11" s="64">
+        <v>43379</v>
+      </c>
       <c r="D11" s="65">
         <v>600</v>
       </c>
@@ -2528,7 +2589,9 @@
         <v>560</v>
       </c>
       <c r="G11" s="56"/>
-      <c r="H11" s="78"/>
+      <c r="H11" s="78">
+        <v>6</v>
+      </c>
       <c r="I11" s="65"/>
       <c r="J11" s="65">
         <v>75</v>
@@ -2543,9 +2606,11 @@
       <c r="O11" s="79"/>
       <c r="P11" s="80"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="52"/>
-      <c r="C12" s="64"/>
+      <c r="C12" s="64">
+        <v>43380</v>
+      </c>
       <c r="D12" s="65"/>
       <c r="E12" s="65">
         <v>245</v>
@@ -2555,7 +2620,9 @@
         <v>315</v>
       </c>
       <c r="G12" s="56"/>
-      <c r="H12" s="78"/>
+      <c r="H12" s="78">
+        <v>7</v>
+      </c>
       <c r="I12" s="65"/>
       <c r="J12" s="65">
         <v>95</v>
@@ -2570,9 +2637,11 @@
       <c r="O12" s="79"/>
       <c r="P12" s="80"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" s="52"/>
-      <c r="C13" s="64"/>
+      <c r="C13" s="64">
+        <v>43381</v>
+      </c>
       <c r="D13" s="65"/>
       <c r="E13" s="65">
         <v>123</v>
@@ -2582,7 +2651,9 @@
         <v>192</v>
       </c>
       <c r="G13" s="56"/>
-      <c r="H13" s="78"/>
+      <c r="H13" s="78">
+        <v>8</v>
+      </c>
       <c r="I13" s="65"/>
       <c r="J13" s="65">
         <v>45</v>
@@ -2597,9 +2668,11 @@
       <c r="O13" s="79"/>
       <c r="P13" s="80"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" s="52"/>
-      <c r="C14" s="64"/>
+      <c r="C14" s="64">
+        <v>43382</v>
+      </c>
       <c r="D14" s="65"/>
       <c r="E14" s="65">
         <v>45</v>
@@ -2609,7 +2682,9 @@
         <v>147</v>
       </c>
       <c r="G14" s="56"/>
-      <c r="H14" s="78"/>
+      <c r="H14" s="78">
+        <v>9</v>
+      </c>
       <c r="I14" s="65"/>
       <c r="J14" s="65"/>
       <c r="K14" s="66">
@@ -2622,9 +2697,11 @@
       <c r="O14" s="79"/>
       <c r="P14" s="80"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" s="52"/>
-      <c r="C15" s="64"/>
+      <c r="C15" s="64">
+        <v>43383</v>
+      </c>
       <c r="D15" s="65"/>
       <c r="E15" s="65">
         <v>79</v>
@@ -2634,7 +2711,9 @@
         <v>68</v>
       </c>
       <c r="G15" s="56"/>
-      <c r="H15" s="78"/>
+      <c r="H15" s="78">
+        <v>10</v>
+      </c>
       <c r="I15" s="65"/>
       <c r="J15" s="65"/>
       <c r="K15" s="66">
@@ -2647,9 +2726,11 @@
       <c r="O15" s="79"/>
       <c r="P15" s="80"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B16" s="52"/>
-      <c r="C16" s="64"/>
+      <c r="C16" s="64">
+        <v>43384</v>
+      </c>
       <c r="D16" s="65">
         <v>600</v>
       </c>
@@ -2661,7 +2742,9 @@
         <v>576</v>
       </c>
       <c r="G16" s="56"/>
-      <c r="H16" s="78"/>
+      <c r="H16" s="78">
+        <v>11</v>
+      </c>
       <c r="I16" s="65"/>
       <c r="J16" s="65"/>
       <c r="K16" s="66">
@@ -2674,9 +2757,11 @@
       <c r="O16" s="79"/>
       <c r="P16" s="80"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" s="52"/>
-      <c r="C17" s="64"/>
+      <c r="C17" s="64">
+        <v>43385</v>
+      </c>
       <c r="D17" s="65"/>
       <c r="E17" s="65">
         <v>235</v>
@@ -2686,7 +2771,9 @@
         <v>341</v>
       </c>
       <c r="G17" s="56"/>
-      <c r="H17" s="78"/>
+      <c r="H17" s="78">
+        <v>12</v>
+      </c>
       <c r="I17" s="65"/>
       <c r="J17" s="65"/>
       <c r="K17" s="66">
@@ -2699,9 +2786,11 @@
       <c r="O17" s="79"/>
       <c r="P17" s="80"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="52"/>
-      <c r="C18" s="64"/>
+      <c r="C18" s="64">
+        <v>43386</v>
+      </c>
       <c r="D18" s="65"/>
       <c r="E18" s="65">
         <v>341</v>
@@ -2711,7 +2800,9 @@
         <v>0</v>
       </c>
       <c r="G18" s="56"/>
-      <c r="H18" s="78"/>
+      <c r="H18" s="78">
+        <v>13</v>
+      </c>
       <c r="I18" s="65"/>
       <c r="J18" s="65"/>
       <c r="K18" s="66">
@@ -2724,9 +2815,11 @@
       <c r="O18" s="79"/>
       <c r="P18" s="80"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="52"/>
-      <c r="C19" s="64"/>
+      <c r="C19" s="64">
+        <v>43387</v>
+      </c>
       <c r="D19" s="65">
         <v>200</v>
       </c>
@@ -2738,7 +2831,9 @@
         <v>77</v>
       </c>
       <c r="G19" s="56"/>
-      <c r="H19" s="76"/>
+      <c r="H19" s="76">
+        <v>14</v>
+      </c>
       <c r="I19" s="65"/>
       <c r="J19" s="65"/>
       <c r="K19" s="66">
@@ -2751,9 +2846,11 @@
       <c r="O19" s="79"/>
       <c r="P19" s="80"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="52"/>
-      <c r="C20" s="67"/>
+      <c r="C20" s="67">
+        <v>43388</v>
+      </c>
       <c r="D20" s="68"/>
       <c r="E20" s="68">
         <v>50</v>
@@ -2784,7 +2881,7 @@
       <c r="O20" s="79"/>
       <c r="P20" s="80"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="52"/>
       <c r="C21" s="56"/>
       <c r="D21" s="56"/>
@@ -2801,7 +2898,7 @@
       <c r="O21" s="79"/>
       <c r="P21" s="80"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="73"/>
       <c r="C22" s="74"/>
       <c r="D22" s="74"/>
@@ -2820,25 +2917,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="16384" width="11.7109375" hidden="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="16" width="11.7265625" customWidth="1"/>
+    <col min="17" max="17" width="3.7265625" customWidth="1"/>
+    <col min="18" max="16384" width="11.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2855,7 +2955,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -2872,7 +2972,7 @@
       <c r="O2" s="15"/>
       <c r="P2" s="16"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="18"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -2889,7 +2989,7 @@
       <c r="O3" s="19"/>
       <c r="P3" s="20"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="21"/>
       <c r="C4" s="32" t="s">
         <v>1</v>
@@ -2910,7 +3010,7 @@
       <c r="O4" s="23"/>
       <c r="P4" s="24"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="21"/>
       <c r="C5" s="34" t="s">
         <v>2</v>
@@ -2941,9 +3041,11 @@
       <c r="O5" s="23"/>
       <c r="P5" s="24"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="21"/>
-      <c r="C6" s="81"/>
+      <c r="C6" s="81" t="s">
+        <v>16</v>
+      </c>
       <c r="D6" s="30">
         <v>187</v>
       </c>
@@ -2970,9 +3072,11 @@
       <c r="O6" s="31"/>
       <c r="P6" s="24"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="21"/>
-      <c r="C7" s="36"/>
+      <c r="C7" s="36" t="s">
+        <v>17</v>
+      </c>
       <c r="D7" s="23">
         <v>998</v>
       </c>
@@ -2999,9 +3103,11 @@
       <c r="O7" s="23"/>
       <c r="P7" s="24"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="21"/>
-      <c r="C8" s="36"/>
+      <c r="C8" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="D8" s="23">
         <v>584</v>
       </c>
@@ -3028,9 +3134,11 @@
       <c r="O8" s="23"/>
       <c r="P8" s="24"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
-      <c r="C9" s="36"/>
+      <c r="C9" s="36" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" s="23">
         <v>917</v>
       </c>
@@ -3057,9 +3165,11 @@
       <c r="O9" s="23"/>
       <c r="P9" s="24"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="21"/>
-      <c r="C10" s="36"/>
+      <c r="C10" s="36" t="s">
+        <v>20</v>
+      </c>
       <c r="D10" s="23">
         <v>155</v>
       </c>
@@ -3086,9 +3196,11 @@
       <c r="O10" s="23"/>
       <c r="P10" s="24"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" s="21"/>
-      <c r="C11" s="36"/>
+      <c r="C11" s="36" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="23">
         <v>452</v>
       </c>
@@ -3115,9 +3227,11 @@
       <c r="O11" s="23"/>
       <c r="P11" s="24"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="21"/>
-      <c r="C12" s="36"/>
+      <c r="C12" s="36" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="23">
         <v>52</v>
       </c>
@@ -3144,9 +3258,11 @@
       <c r="O12" s="23"/>
       <c r="P12" s="24"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" s="21"/>
-      <c r="C13" s="36"/>
+      <c r="C13" s="36" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" s="23">
         <v>975</v>
       </c>
@@ -3173,9 +3289,11 @@
       <c r="O13" s="23"/>
       <c r="P13" s="24"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" s="21"/>
-      <c r="C14" s="36"/>
+      <c r="C14" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="D14" s="23">
         <v>705</v>
       </c>
@@ -3202,9 +3320,11 @@
       <c r="O14" s="23"/>
       <c r="P14" s="24"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" s="21"/>
-      <c r="C15" s="36"/>
+      <c r="C15" s="36" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="23">
         <v>369</v>
       </c>
@@ -3231,9 +3351,11 @@
       <c r="O15" s="23"/>
       <c r="P15" s="24"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B16" s="21"/>
-      <c r="C16" s="36"/>
+      <c r="C16" s="36" t="s">
+        <v>26</v>
+      </c>
       <c r="D16" s="23">
         <v>84</v>
       </c>
@@ -3260,9 +3382,11 @@
       <c r="O16" s="23"/>
       <c r="P16" s="24"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" s="21"/>
-      <c r="C17" s="38"/>
+      <c r="C17" s="38" t="s">
+        <v>27</v>
+      </c>
       <c r="D17" s="26">
         <v>982</v>
       </c>
@@ -3289,7 +3413,7 @@
       <c r="O17" s="23"/>
       <c r="P17" s="24"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="21"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -3306,7 +3430,7 @@
       <c r="O18" s="23"/>
       <c r="P18" s="24"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="21"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
@@ -3323,7 +3447,7 @@
       <c r="O19" s="23"/>
       <c r="P19" s="24"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="21"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
@@ -3340,7 +3464,7 @@
       <c r="O20" s="23"/>
       <c r="P20" s="24"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="21"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
@@ -3357,7 +3481,7 @@
       <c r="O21" s="23"/>
       <c r="P21" s="24"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>

</xml_diff>